<commit_message>
added data from DC feb summit
</commit_message>
<xml_diff>
--- a/3-13-12/testingData.xlsx
+++ b/3-13-12/testingData.xlsx
@@ -286,11 +286,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="672738488"/>
-        <c:axId val="672745272"/>
+        <c:axId val="639264424"/>
+        <c:axId val="170155576"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="672738488"/>
+        <c:axId val="639264424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -318,7 +318,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="672745272"/>
+        <c:crossAx val="170155576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -326,7 +326,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="672745272"/>
+        <c:axId val="170155576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -360,7 +360,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="672738488"/>
+        <c:crossAx val="639264424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -535,11 +535,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="672809352"/>
-        <c:axId val="672815016"/>
+        <c:axId val="639248184"/>
+        <c:axId val="639224504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="672809352"/>
+        <c:axId val="639248184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,7 +572,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="672815016"/>
+        <c:crossAx val="639224504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -580,7 +580,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="672815016"/>
+        <c:axId val="639224504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -610,7 +610,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="672809352"/>
+        <c:crossAx val="639248184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -780,11 +780,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="672845928"/>
-        <c:axId val="672851368"/>
+        <c:axId val="639093352"/>
+        <c:axId val="638841064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="672845928"/>
+        <c:axId val="639093352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,7 +812,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="672851368"/>
+        <c:crossAx val="638841064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -820,7 +820,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="672851368"/>
+        <c:axId val="638841064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -850,7 +850,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="672845928"/>
+        <c:crossAx val="639093352"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>

</xml_diff>